<commit_message>
Ajout Buzzer + main
</commit_message>
<xml_diff>
--- a/Objectif.xlsx
+++ b/Objectif.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5636f4ccf65991be/Bureau/lycee/2025 - INSA - S7/C^M^M/BE_POO_MILI_BENAMOR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{8FC71A0B-2A32-417B-8A50-86E01EF247C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A53B733-D8DD-4BBC-81C4-00E38F152C57}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="8_{8FC71A0B-2A32-417B-8A50-86E01EF247C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D43960A-179F-4BD5-8809-95C38FE13AA6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8705E0E3-F7CB-4D4B-9586-AB6CBCF6D11D}"/>
   </bookViews>
   <sheets>
     <sheet name="Objectifs" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="UML" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>Objectif</t>
   </si>
@@ -145,6 +145,18 @@
   </si>
   <si>
     <t>Code de sécurité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Progres </t>
+  </si>
+  <si>
+    <t>Classe detection mouvement réalisée</t>
+  </si>
+  <si>
+    <t>Porte</t>
+  </si>
+  <si>
+    <t>à tester</t>
   </si>
 </sst>
 </file>
@@ -313,15 +325,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0A3BFC1B-20E8-4850-AD27-C343C6C7CE3C}" name="Table1" displayName="Table1" ref="A1:F1048575" totalsRowShown="0">
-  <autoFilter ref="A1:F1048575" xr:uid="{0A3BFC1B-20E8-4850-AD27-C343C6C7CE3C}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0A3BFC1B-20E8-4850-AD27-C343C6C7CE3C}" name="Table1" displayName="Table1" ref="A1:G1048575" totalsRowShown="0">
+  <autoFilter ref="A1:G1048575" xr:uid="{0A3BFC1B-20E8-4850-AD27-C343C6C7CE3C}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{9C41B17B-1BC4-446A-8725-CEE113B38E07}" name="Objectif"/>
     <tableColumn id="2" xr3:uid="{9870D0D2-FA91-4727-97E1-FF2C81DC00E1}" name="Composants"/>
     <tableColumn id="3" xr3:uid="{3475FE33-03CD-4508-830E-B39FC8A04627}" name="details"/>
     <tableColumn id="4" xr3:uid="{99C59C18-6E03-439F-B5E8-ECF1748573FF}" name="Column4"/>
     <tableColumn id="5" xr3:uid="{F477D3A5-79D4-426F-B354-453F1F4E84AB}" name="fait ?"/>
     <tableColumn id="6" xr3:uid="{E9FBC7C1-EB3A-462C-BDCD-CE1E12D1710D}" name="Programmeur"/>
+    <tableColumn id="7" xr3:uid="{CECD9FBB-D706-44F3-82BC-E7CB9C5C7E1C}" name="Progres "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -644,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99E08C89-BF84-4EF4-A896-EBE0A22D53F8}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,9 +670,10 @@
     <col min="3" max="3" width="63" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.33203125" customWidth="1"/>
     <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -678,8 +692,11 @@
       <c r="F1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -695,8 +712,11 @@
       <c r="F2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -707,13 +727,16 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -730,7 +753,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -747,7 +770,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -761,12 +784,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -777,7 +800,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -812,10 +835,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AEE26CB-4CD5-43AC-8B1D-0B6C6616E8E8}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,7 +849,7 @@
     <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -834,7 +857,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -846,6 +869,9 @@
       </c>
       <c r="D2" t="s">
         <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout Buzzer + main testé
</commit_message>
<xml_diff>
--- a/Objectif.xlsx
+++ b/Objectif.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5636f4ccf65991be/Bureau/lycee/2025 - INSA - S7/C^M^M/BE_POO_MILI_BENAMOR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{8FC71A0B-2A32-417B-8A50-86E01EF247C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D43960A-179F-4BD5-8809-95C38FE13AA6}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{8FC71A0B-2A32-417B-8A50-86E01EF247C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1303EA71-1BD9-41E5-9DDD-856C6A2D2096}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8705E0E3-F7CB-4D4B-9586-AB6CBCF6D11D}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12204" xr2:uid="{8705E0E3-F7CB-4D4B-9586-AB6CBCF6D11D}"/>
   </bookViews>
   <sheets>
     <sheet name="Objectifs" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>Objectif</t>
   </si>
@@ -102,6 +102,9 @@
     <t>Column4</t>
   </si>
   <si>
+    <t>Oui</t>
+  </si>
+  <si>
     <t>En cours</t>
   </si>
   <si>
@@ -156,7 +159,7 @@
     <t>Porte</t>
   </si>
   <si>
-    <t>à tester</t>
+    <t>validé</t>
   </si>
 </sst>
 </file>
@@ -660,7 +663,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -690,10 +693,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -707,13 +710,13 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -730,10 +733,10 @@
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -750,7 +753,7 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -764,21 +767,21 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -802,10 +805,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
@@ -851,27 +854,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout detection de mouvement fonctionnelle avec porte testés
</commit_message>
<xml_diff>
--- a/Objectif.xlsx
+++ b/Objectif.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5636f4ccf65991be/Bureau/lycee/2025 - INSA - S7/C^M^M/BE_POO_MILI_BENAMOR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{8FC71A0B-2A32-417B-8A50-86E01EF247C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1303EA71-1BD9-41E5-9DDD-856C6A2D2096}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{8FC71A0B-2A32-417B-8A50-86E01EF247C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4522CF25-4BCF-42C6-B66F-95D50FACFF12}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12204" xr2:uid="{8705E0E3-F7CB-4D4B-9586-AB6CBCF6D11D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8705E0E3-F7CB-4D4B-9586-AB6CBCF6D11D}"/>
   </bookViews>
   <sheets>
     <sheet name="Objectifs" sheetId="1" r:id="rId1"/>
@@ -663,7 +663,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,7 +750,7 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
         <v>25</v>

</xml_diff>